<commit_message>
Change the building of the context.
Change the building of the context to build it from the variables used in excel file.
</commit_message>
<xml_diff>
--- a/tests/Payroll/repository/truth-table.xlsx
+++ b/tests/Payroll/repository/truth-table.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="205" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -35,6 +34,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -120,17 +120,17 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -138,7 +138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -146,7 +146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="1" t="n">
         <v>0</v>
       </c>
@@ -154,7 +154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
@@ -162,7 +162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
@@ -186,44 +186,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
At support for logger
One logger to be used by the repository of rules are added.
</commit_message>
<xml_diff>
--- a/tests/Payroll/repository/truth-table.xlsx
+++ b/tests/Payroll/repository/truth-table.xlsx
@@ -5,23 +5,30 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="273" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TruthTable" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TruthTableGenerated" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>P</t>
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -96,9 +103,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -120,54 +130,54 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0</v>
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1</v>
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -186,17 +196,85 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
@@ -204,7 +282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -212,7 +290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -220,7 +298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Improve Repository interface and tests
Cahnged the RuleRepository to take into account technical issues
when evaluating rules. Added more tests and another Repository, this
one generated by the dsl tool. Add logger for testng purposes when
firing the rules action.
</commit_message>
<xml_diff>
--- a/tests/Payroll/repository/truth-table.xlsx
+++ b/tests/Payroll/repository/truth-table.xlsx
@@ -5,23 +5,30 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="194" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="273" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TruthTable" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TruthTableGenerated" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>P</t>
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -96,9 +103,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -120,54 +130,54 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0</v>
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1</v>
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -186,17 +196,85 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
@@ -204,7 +282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -212,7 +290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -220,7 +298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>

</xml_diff>